<commit_message>
updating app for things
</commit_message>
<xml_diff>
--- a/COVIDPPP/regressors.xlsx
+++ b/COVIDPPP/regressors.xlsx
@@ -1,52 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Justin\Gov50\pppdata\COVIDPPP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Regular/Desktop/GOV50/pppdata/COVIDPPP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CB7C62-C6E6-4D8E-AAA4-DADA6C8AF284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF0DFD1-631B-B24B-8909-AC37A33AAE30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFADD8B4-DA0F-4AD7-B952-63B27F847954}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="26400" windowHeight="14900" xr2:uid="{AFADD8B4-DA0F-4AD7-B952-63B27F847954}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="85">
   <si>
     <t>Variable name</t>
   </si>
   <si>
     <t>Definition</t>
-  </si>
-  <si>
-    <t>days_to_approval</t>
-  </si>
-  <si>
-    <t>Days from date applications opened to date approved</t>
   </si>
   <si>
     <t xml:space="preserve">median_family_income </t>
@@ -296,6 +281,18 @@
   </si>
   <si>
     <t>Non-white as percent of population</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>Whether loan was approved after PPP first ran out of money (April 16, 2020)</t>
+  </si>
+  <si>
+    <t>business_days</t>
+  </si>
+  <si>
+    <t>Business days from date applications opened to date approved</t>
   </si>
 </sst>
 </file>
@@ -386,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -401,6 +398,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -717,19 +717,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CAA409-C6EA-4FDE-A6B3-570889C837DD}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="2" width="64.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -737,292 +737,300 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B25" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="5"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A30:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1031,19 +1039,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B217914-E4F4-4883-A30C-C8D30F0E09BD}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" customWidth="1"/>
-    <col min="2" max="2" width="42.44140625" customWidth="1"/>
+    <col min="1" max="1" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1051,292 +1059,300 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="B6" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B25" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="5"/>
+    </row>
+    <row r="31" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="B31" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="B35" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="37" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+    <row r="38" spans="1:2" ht="28" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A30:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>